<commit_message>
first wkg live push version
</commit_message>
<xml_diff>
--- a/excel_templates/parceltariff.xlsx
+++ b/excel_templates/parceltariff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtse\Documents\Python Scripts\epg wkg\2022-08-10 Rate Card Flask Demo\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtse\source\Workspaces\QuoteTestApp\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEE7CDA-FC71-4F73-B5A1-F06E533EFD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244994A0-D179-42A9-BCC0-2CF99E20CDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46CACC1E-1B77-46EB-83A0-CFA944E72F12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{46CACC1E-1B77-46EB-83A0-CFA944E72F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="8" r:id="rId1"/>
@@ -3009,7 +3009,7 @@
   </sheetPr>
   <dimension ref="A1:AI24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
@@ -4763,19 +4763,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717C4292-31F6-45CC-ABA5-E4C40A83A247}">
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="16384" width="13.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>